<commit_message>
added manager info name columns in all tabs, nothing more
</commit_message>
<xml_diff>
--- a/Source Data/Active Beneficiary Data - Eveningstar.xlsx
+++ b/Source Data/Active Beneficiary Data - Eveningstar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D DRIVE\JK_SOFT_PROJECTS\morning_star\Source Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC2C32F-24A1-4126-9264-11C9B6C42A6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF0305C-AD98-4897-BBA7-EB7E47DA633F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17563" windowHeight="6120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17563" windowHeight="6120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ActiveBeneficiaryData-Mo" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2463" uniqueCount="771">
   <si>
     <t>Case No</t>
   </si>
@@ -3208,11 +3208,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO183"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AH3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH2" sqref="AH2"/>
+      <selection pane="bottomRight" activeCell="AH3" sqref="AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.8" x14ac:dyDescent="0.3"/>
@@ -3463,8 +3463,12 @@
       <c r="AG2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
+      <c r="AH2" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
       <c r="AL2" s="3"/>
@@ -3552,8 +3556,12 @@
       <c r="AG3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AH3" s="3"/>
-      <c r="AI3" s="3"/>
+      <c r="AH3" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ3" s="3"/>
       <c r="AK3" s="3"/>
       <c r="AL3" s="3"/>
@@ -3629,8 +3637,12 @@
       <c r="AG4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AH4" s="3"/>
-      <c r="AI4" s="3"/>
+      <c r="AH4" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ4" s="3"/>
       <c r="AK4" s="3"/>
       <c r="AL4" s="3"/>
@@ -3716,8 +3728,12 @@
       <c r="AG5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH5" s="3"/>
-      <c r="AI5" s="3"/>
+      <c r="AH5" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
       <c r="AL5" s="3"/>
@@ -3795,8 +3811,12 @@
       <c r="AG6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="3"/>
+      <c r="AH6" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ6" s="3"/>
       <c r="AK6" s="3"/>
       <c r="AL6" s="3"/>
@@ -3860,8 +3880,12 @@
         <v>67</v>
       </c>
       <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
-      <c r="AI7" s="3"/>
+      <c r="AH7" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ7" s="3">
         <v>100006</v>
       </c>
@@ -3939,8 +3963,12 @@
         <v>64</v>
       </c>
       <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
+      <c r="AH8" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ8" s="3">
         <v>100007</v>
       </c>
@@ -4016,8 +4044,12 @@
       <c r="AE9" s="3"/>
       <c r="AF9" s="3"/>
       <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
-      <c r="AI9" s="3"/>
+      <c r="AH9" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI9" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ9" s="3">
         <v>100008</v>
       </c>
@@ -4111,8 +4143,12 @@
       <c r="AG10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
+      <c r="AH10" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI10" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ10" s="3">
         <v>100009</v>
       </c>
@@ -4200,8 +4236,12 @@
       <c r="AG11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH11" s="3"/>
-      <c r="AI11" s="3"/>
+      <c r="AH11" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI11" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ11" s="3">
         <v>100010</v>
       </c>
@@ -4279,8 +4319,12 @@
       <c r="AG12" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AH12" s="3"/>
-      <c r="AI12" s="3"/>
+      <c r="AH12" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI12" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ12" s="3">
         <v>100011</v>
       </c>
@@ -4370,8 +4414,12 @@
       <c r="AG13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH13" s="3"/>
-      <c r="AI13" s="3"/>
+      <c r="AH13" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI13" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ13" s="3">
         <v>100012</v>
       </c>
@@ -4459,8 +4507,12 @@
       <c r="AG14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH14" s="3"/>
-      <c r="AI14" s="3"/>
+      <c r="AH14" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI14" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ14" s="3">
         <v>100013</v>
       </c>
@@ -4548,8 +4600,12 @@
       </c>
       <c r="AF15" s="3"/>
       <c r="AG15" s="3"/>
-      <c r="AH15" s="3"/>
-      <c r="AI15" s="3"/>
+      <c r="AH15" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI15" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ15" s="3">
         <v>100014</v>
       </c>
@@ -4629,8 +4685,12 @@
       <c r="AE16" s="3"/>
       <c r="AF16" s="3"/>
       <c r="AG16" s="3"/>
-      <c r="AH16" s="3"/>
-      <c r="AI16" s="3"/>
+      <c r="AH16" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI16" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ16" s="3">
         <v>100015</v>
       </c>
@@ -4714,8 +4774,12 @@
       <c r="AG17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH17" s="3"/>
-      <c r="AI17" s="3"/>
+      <c r="AH17" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI17" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ17" s="3">
         <v>100016</v>
       </c>
@@ -4793,8 +4857,12 @@
         <v>90</v>
       </c>
       <c r="AG18" s="3"/>
-      <c r="AH18" s="3"/>
-      <c r="AI18" s="3"/>
+      <c r="AH18" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI18" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ18" s="3">
         <v>100017</v>
       </c>
@@ -4868,8 +4936,12 @@
       <c r="AE19" s="3"/>
       <c r="AF19" s="3"/>
       <c r="AG19" s="3"/>
-      <c r="AH19" s="3"/>
-      <c r="AI19" s="3"/>
+      <c r="AH19" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI19" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ19" s="3">
         <v>100018</v>
       </c>
@@ -4949,8 +5021,12 @@
       <c r="AE20" s="3"/>
       <c r="AF20" s="3"/>
       <c r="AG20" s="3"/>
-      <c r="AH20" s="3"/>
-      <c r="AI20" s="3"/>
+      <c r="AH20" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI20" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ20" s="3">
         <v>100019</v>
       </c>
@@ -5036,8 +5112,12 @@
       </c>
       <c r="AF21" s="3"/>
       <c r="AG21" s="3"/>
-      <c r="AH21" s="3"/>
-      <c r="AI21" s="3"/>
+      <c r="AH21" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI21" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ21" s="3">
         <v>100020</v>
       </c>
@@ -5115,8 +5195,12 @@
         <v>90</v>
       </c>
       <c r="AG22" s="3"/>
-      <c r="AH22" s="3"/>
-      <c r="AI22" s="3"/>
+      <c r="AH22" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI22" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ22" s="3">
         <v>100021</v>
       </c>
@@ -5210,8 +5294,12 @@
       <c r="AG23" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AH23" s="3"/>
-      <c r="AI23" s="3"/>
+      <c r="AH23" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI23" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ23" s="3">
         <v>100022</v>
       </c>
@@ -5299,8 +5387,12 @@
       <c r="AG24" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH24" s="3"/>
-      <c r="AI24" s="3"/>
+      <c r="AH24" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI24" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ24" s="3">
         <v>100023</v>
       </c>
@@ -5386,8 +5478,12 @@
       <c r="AG25" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH25" s="3"/>
-      <c r="AI25" s="3"/>
+      <c r="AH25" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI25" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ25" s="3">
         <v>100024</v>
       </c>
@@ -5477,8 +5573,12 @@
       <c r="AG26" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH26" s="3"/>
-      <c r="AI26" s="3"/>
+      <c r="AH26" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI26" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ26" s="3">
         <v>100025</v>
       </c>
@@ -5558,8 +5658,12 @@
       <c r="AG27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AH27" s="3"/>
-      <c r="AI27" s="3"/>
+      <c r="AH27" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI27" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ27" s="3">
         <v>100026</v>
       </c>
@@ -5651,8 +5755,12 @@
       <c r="AG28" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH28" s="3"/>
-      <c r="AI28" s="3"/>
+      <c r="AH28" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI28" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ28" s="3">
         <v>100027</v>
       </c>
@@ -5738,8 +5846,12 @@
       <c r="AG29" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="AH29" s="3"/>
-      <c r="AI29" s="3"/>
+      <c r="AH29" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI29" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ29" s="3">
         <v>100028</v>
       </c>
@@ -5829,8 +5941,12 @@
       <c r="AG30" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="AH30" s="3"/>
-      <c r="AI30" s="3"/>
+      <c r="AH30" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI30" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ30" s="3">
         <v>100029</v>
       </c>
@@ -5916,8 +6032,12 @@
       <c r="AG31" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH31" s="3"/>
-      <c r="AI31" s="3"/>
+      <c r="AH31" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI31" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ31" s="3">
         <v>100030</v>
       </c>
@@ -6003,8 +6123,12 @@
       <c r="AG32" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH32" s="3"/>
-      <c r="AI32" s="3"/>
+      <c r="AH32" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI32" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ32" s="3">
         <v>100031</v>
       </c>
@@ -6094,8 +6218,12 @@
       <c r="AG33" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="AH33" s="3"/>
-      <c r="AI33" s="3"/>
+      <c r="AH33" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI33" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ33" s="3">
         <v>100032</v>
       </c>
@@ -6173,8 +6301,12 @@
         <v>120</v>
       </c>
       <c r="AG34" s="3"/>
-      <c r="AH34" s="3"/>
-      <c r="AI34" s="3"/>
+      <c r="AH34" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI34" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ34" s="3">
         <v>100033</v>
       </c>
@@ -6266,8 +6398,12 @@
       <c r="AG35" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH35" s="3"/>
-      <c r="AI35" s="3"/>
+      <c r="AH35" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI35" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ35" s="3">
         <v>100034</v>
       </c>
@@ -6363,8 +6499,12 @@
       <c r="AG36" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH36" s="3"/>
-      <c r="AI36" s="3"/>
+      <c r="AH36" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI36" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ36" s="3">
         <v>100035</v>
       </c>
@@ -6440,8 +6580,12 @@
       <c r="AE37" s="3"/>
       <c r="AF37" s="3"/>
       <c r="AG37" s="3"/>
-      <c r="AH37" s="3"/>
-      <c r="AI37" s="3"/>
+      <c r="AH37" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI37" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ37" s="3">
         <v>100036</v>
       </c>
@@ -6521,8 +6665,12 @@
       <c r="AG38" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH38" s="3"/>
-      <c r="AI38" s="3"/>
+      <c r="AH38" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI38" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ38" s="3">
         <v>100037</v>
       </c>
@@ -6614,8 +6762,12 @@
       <c r="AG39" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH39" s="3"/>
-      <c r="AI39" s="3"/>
+      <c r="AH39" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI39" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ39" s="3">
         <v>100038</v>
       </c>
@@ -6695,8 +6847,12 @@
       <c r="AE40" s="3"/>
       <c r="AF40" s="3"/>
       <c r="AG40" s="3"/>
-      <c r="AH40" s="3"/>
-      <c r="AI40" s="3"/>
+      <c r="AH40" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI40" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ40" s="3">
         <v>100039</v>
       </c>
@@ -6784,8 +6940,12 @@
       <c r="AG41" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AH41" s="3"/>
-      <c r="AI41" s="3"/>
+      <c r="AH41" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI41" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ41" s="3">
         <v>100040</v>
       </c>
@@ -6875,8 +7035,12 @@
       <c r="AG42" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH42" s="3"/>
-      <c r="AI42" s="3"/>
+      <c r="AH42" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI42" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ42" s="3">
         <v>100041</v>
       </c>
@@ -6960,8 +7124,12 @@
       <c r="AG43" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH43" s="3"/>
-      <c r="AI43" s="3"/>
+      <c r="AH43" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI43" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ43" s="3">
         <v>100042</v>
       </c>
@@ -7047,8 +7215,12 @@
       <c r="AG44" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH44" s="3"/>
-      <c r="AI44" s="3"/>
+      <c r="AH44" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI44" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ44" s="3">
         <v>100043</v>
       </c>
@@ -7126,8 +7298,12 @@
       <c r="AE45" s="3"/>
       <c r="AF45" s="3"/>
       <c r="AG45" s="3"/>
-      <c r="AH45" s="3"/>
-      <c r="AI45" s="3"/>
+      <c r="AH45" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI45" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ45" s="3">
         <v>100044</v>
       </c>
@@ -7205,8 +7381,12 @@
       <c r="AE46" s="3"/>
       <c r="AF46" s="3"/>
       <c r="AG46" s="3"/>
-      <c r="AH46" s="3"/>
-      <c r="AI46" s="3"/>
+      <c r="AH46" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI46" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ46" s="3">
         <v>100045</v>
       </c>
@@ -7286,8 +7466,12 @@
       <c r="AG47" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="AH47" s="3"/>
-      <c r="AI47" s="3"/>
+      <c r="AH47" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI47" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ47" s="3">
         <v>100046</v>
       </c>
@@ -7369,8 +7553,12 @@
       <c r="AG48" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH48" s="3"/>
-      <c r="AI48" s="3"/>
+      <c r="AH48" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI48" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ48" s="3">
         <v>100047</v>
       </c>
@@ -7466,8 +7654,12 @@
       <c r="AG49" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="AH49" s="3"/>
-      <c r="AI49" s="3"/>
+      <c r="AH49" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI49" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ49" s="3">
         <v>100048</v>
       </c>
@@ -7557,8 +7749,12 @@
       <c r="AG50" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH50" s="3"/>
-      <c r="AI50" s="3"/>
+      <c r="AH50" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI50" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ50" s="3">
         <v>100049</v>
       </c>
@@ -7640,8 +7836,12 @@
       <c r="AG51" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AH51" s="3"/>
-      <c r="AI51" s="3"/>
+      <c r="AH51" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI51" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ51" s="3">
         <v>100050</v>
       </c>
@@ -7723,8 +7923,12 @@
       <c r="AG52" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH52" s="3"/>
-      <c r="AI52" s="3"/>
+      <c r="AH52" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI52" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ52" s="3">
         <v>100051</v>
       </c>
@@ -7800,8 +8004,12 @@
       <c r="AE53" s="3"/>
       <c r="AF53" s="3"/>
       <c r="AG53" s="3"/>
-      <c r="AH53" s="3"/>
-      <c r="AI53" s="3"/>
+      <c r="AH53" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI53" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ53" s="3">
         <v>100052</v>
       </c>
@@ -7881,8 +8089,12 @@
       <c r="AG54" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH54" s="3"/>
-      <c r="AI54" s="3"/>
+      <c r="AH54" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI54" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ54" s="3">
         <v>100053</v>
       </c>
@@ -7966,8 +8178,12 @@
       <c r="AG55" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH55" s="3"/>
-      <c r="AI55" s="3"/>
+      <c r="AH55" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI55" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ55" s="3">
         <v>100054</v>
       </c>
@@ -8047,8 +8263,12 @@
       <c r="AG56" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH56" s="3"/>
-      <c r="AI56" s="3"/>
+      <c r="AH56" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI56" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ56" s="3">
         <v>100055</v>
       </c>
@@ -8128,8 +8348,12 @@
       <c r="AG57" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH57" s="3"/>
-      <c r="AI57" s="3"/>
+      <c r="AH57" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI57" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ57" s="3">
         <v>100056</v>
       </c>
@@ -8219,8 +8443,12 @@
       <c r="AG58" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH58" s="3"/>
-      <c r="AI58" s="3"/>
+      <c r="AH58" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI58" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ58" s="3">
         <v>100057</v>
       </c>
@@ -8308,8 +8536,12 @@
       <c r="AG59" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="AH59" s="3"/>
-      <c r="AI59" s="3"/>
+      <c r="AH59" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI59" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ59" s="3">
         <v>100058</v>
       </c>
@@ -8385,8 +8617,12 @@
       <c r="AE60" s="3"/>
       <c r="AF60" s="3"/>
       <c r="AG60" s="3"/>
-      <c r="AH60" s="3"/>
-      <c r="AI60" s="3"/>
+      <c r="AH60" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI60" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ60" s="3">
         <v>100059</v>
       </c>
@@ -8474,8 +8710,12 @@
       <c r="AG61" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="AH61" s="3"/>
-      <c r="AI61" s="3"/>
+      <c r="AH61" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI61" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ61" s="3">
         <v>100060</v>
       </c>
@@ -8565,8 +8805,12 @@
       <c r="AG62" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH62" s="3"/>
-      <c r="AI62" s="3"/>
+      <c r="AH62" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI62" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ62" s="3">
         <v>100061</v>
       </c>
@@ -8654,8 +8898,12 @@
       <c r="AG63" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="AH63" s="3"/>
-      <c r="AI63" s="3"/>
+      <c r="AH63" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI63" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ63" s="3">
         <v>100062</v>
       </c>
@@ -8741,8 +8989,12 @@
       </c>
       <c r="AF64" s="3"/>
       <c r="AG64" s="3"/>
-      <c r="AH64" s="3"/>
-      <c r="AI64" s="3"/>
+      <c r="AH64" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI64" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ64" s="3">
         <v>100063</v>
       </c>
@@ -8830,8 +9082,12 @@
       <c r="AG65" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH65" s="3"/>
-      <c r="AI65" s="3"/>
+      <c r="AH65" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI65" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ65" s="3">
         <v>100064</v>
       </c>
@@ -8921,8 +9177,12 @@
       <c r="AG66" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="AH66" s="3"/>
-      <c r="AI66" s="3"/>
+      <c r="AH66" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI66" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ66" s="3">
         <v>100065</v>
       </c>
@@ -8996,8 +9256,12 @@
       <c r="AE67" s="3"/>
       <c r="AF67" s="3"/>
       <c r="AG67" s="3"/>
-      <c r="AH67" s="3"/>
-      <c r="AI67" s="3"/>
+      <c r="AH67" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI67" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ67" s="3">
         <v>100066</v>
       </c>
@@ -9073,8 +9337,12 @@
       <c r="AE68" s="3"/>
       <c r="AF68" s="3"/>
       <c r="AG68" s="3"/>
-      <c r="AH68" s="3"/>
-      <c r="AI68" s="3"/>
+      <c r="AH68" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI68" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ68" s="3">
         <v>100067</v>
       </c>
@@ -9162,8 +9430,12 @@
       <c r="AG69" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="AH69" s="3"/>
-      <c r="AI69" s="3"/>
+      <c r="AH69" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI69" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ69" s="3">
         <v>100068</v>
       </c>
@@ -9239,8 +9511,12 @@
       <c r="AG70" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="AH70" s="3"/>
-      <c r="AI70" s="3"/>
+      <c r="AH70" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI70" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ70" s="3">
         <v>100069</v>
       </c>
@@ -9320,8 +9596,12 @@
       <c r="AG71" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AH71" s="3"/>
-      <c r="AI71" s="3"/>
+      <c r="AH71" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI71" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ71" s="3">
         <v>100070</v>
       </c>
@@ -9411,8 +9691,12 @@
       <c r="AG72" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="AH72" s="3"/>
-      <c r="AI72" s="3"/>
+      <c r="AH72" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI72" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ72" s="3">
         <v>100071</v>
       </c>
@@ -9480,8 +9764,12 @@
       <c r="AG73" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="AH73" s="3"/>
-      <c r="AI73" s="3"/>
+      <c r="AH73" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI73" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ73" s="3">
         <v>100072</v>
       </c>
@@ -9559,8 +9847,12 @@
       <c r="AE74" s="3"/>
       <c r="AF74" s="3"/>
       <c r="AG74" s="3"/>
-      <c r="AH74" s="3"/>
-      <c r="AI74" s="3"/>
+      <c r="AH74" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI74" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ74" s="3">
         <v>100073</v>
       </c>
@@ -9646,8 +9938,12 @@
       <c r="AG75" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH75" s="3"/>
-      <c r="AI75" s="3"/>
+      <c r="AH75" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI75" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ75" s="3">
         <v>100074</v>
       </c>
@@ -9727,8 +10023,12 @@
       <c r="AG76" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH76" s="3"/>
-      <c r="AI76" s="3"/>
+      <c r="AH76" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI76" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ76" s="3">
         <v>100075</v>
       </c>
@@ -9814,8 +10114,12 @@
       <c r="AG77" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH77" s="3"/>
-      <c r="AI77" s="3"/>
+      <c r="AH77" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI77" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ77" s="3">
         <v>100076</v>
       </c>
@@ -9905,8 +10209,12 @@
       <c r="AG78" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="AH78" s="3"/>
-      <c r="AI78" s="3"/>
+      <c r="AH78" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI78" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ78" s="3">
         <v>100077</v>
       </c>
@@ -9982,8 +10290,12 @@
       <c r="AG79" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="AH79" s="3"/>
-      <c r="AI79" s="3"/>
+      <c r="AH79" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI79" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ79" s="3">
         <v>100078</v>
       </c>
@@ -10073,8 +10385,12 @@
       <c r="AG80" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="AH80" s="3"/>
-      <c r="AI80" s="3"/>
+      <c r="AH80" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI80" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ80" s="3">
         <v>100079</v>
       </c>
@@ -10144,8 +10460,12 @@
         <v>232</v>
       </c>
       <c r="AG81" s="3"/>
-      <c r="AH81" s="3"/>
-      <c r="AI81" s="3"/>
+      <c r="AH81" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI81" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ81" s="3">
         <v>100080</v>
       </c>
@@ -10219,8 +10539,12 @@
       <c r="AG82" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH82" s="3"/>
-      <c r="AI82" s="3"/>
+      <c r="AH82" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI82" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ82" s="3">
         <v>100081</v>
       </c>
@@ -10310,8 +10634,12 @@
       <c r="AG83" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH83" s="3"/>
-      <c r="AI83" s="3"/>
+      <c r="AH83" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI83" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ83" s="3">
         <v>100082</v>
       </c>
@@ -10385,8 +10713,12 @@
       <c r="AG84" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AH84" s="3"/>
-      <c r="AI84" s="3"/>
+      <c r="AH84" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI84" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ84" s="3">
         <v>100083</v>
       </c>
@@ -10464,8 +10796,12 @@
       <c r="AG85" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="AH85" s="3"/>
-      <c r="AI85" s="3"/>
+      <c r="AH85" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI85" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ85" s="3">
         <v>100084</v>
       </c>
@@ -10559,8 +10895,12 @@
       <c r="AG86" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH86" s="3"/>
-      <c r="AI86" s="3"/>
+      <c r="AH86" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI86" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ86" s="3">
         <v>100085</v>
       </c>
@@ -10658,8 +10998,12 @@
       <c r="AG87" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH87" s="3"/>
-      <c r="AI87" s="3"/>
+      <c r="AH87" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI87" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ87" s="3">
         <v>100086</v>
       </c>
@@ -10735,8 +11079,12 @@
       <c r="AE88" s="3"/>
       <c r="AF88" s="3"/>
       <c r="AG88" s="3"/>
-      <c r="AH88" s="3"/>
-      <c r="AI88" s="3"/>
+      <c r="AH88" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI88" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ88" s="3">
         <v>100087</v>
       </c>
@@ -10816,8 +11164,12 @@
       <c r="AG89" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="AH89" s="3"/>
-      <c r="AI89" s="3"/>
+      <c r="AH89" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI89" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ89" s="3">
         <v>100088</v>
       </c>
@@ -10905,8 +11257,12 @@
       <c r="AG90" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH90" s="3"/>
-      <c r="AI90" s="3"/>
+      <c r="AH90" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI90" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ90" s="3">
         <v>100089</v>
       </c>
@@ -10982,8 +11338,12 @@
       <c r="AE91" s="3"/>
       <c r="AF91" s="3"/>
       <c r="AG91" s="3"/>
-      <c r="AH91" s="3"/>
-      <c r="AI91" s="3"/>
+      <c r="AH91" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI91" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ91" s="3">
         <v>100090</v>
       </c>
@@ -11043,8 +11403,12 @@
         <v>67</v>
       </c>
       <c r="AG92" s="3"/>
-      <c r="AH92" s="3"/>
-      <c r="AI92" s="3"/>
+      <c r="AH92" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI92" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ92" s="3">
         <v>100091</v>
       </c>
@@ -11132,8 +11496,12 @@
       <c r="AG93" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="AH93" s="3"/>
-      <c r="AI93" s="3"/>
+      <c r="AH93" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI93" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ93" s="3">
         <v>100092</v>
       </c>
@@ -11215,8 +11583,12 @@
       <c r="AG94" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AH94" s="3"/>
-      <c r="AI94" s="3"/>
+      <c r="AH94" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI94" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ94" s="3">
         <v>100093</v>
       </c>
@@ -11302,8 +11674,12 @@
       </c>
       <c r="AF95" s="3"/>
       <c r="AG95" s="3"/>
-      <c r="AH95" s="3"/>
-      <c r="AI95" s="3"/>
+      <c r="AH95" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI95" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ95" s="3">
         <v>100094</v>
       </c>
@@ -11381,8 +11757,12 @@
       <c r="AG96" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="AH96" s="3"/>
-      <c r="AI96" s="3"/>
+      <c r="AH96" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI96" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ96" s="3">
         <v>100095</v>
       </c>
@@ -11472,8 +11852,12 @@
       <c r="AG97" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH97" s="3"/>
-      <c r="AI97" s="3"/>
+      <c r="AH97" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI97" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ97" s="3">
         <v>100096</v>
       </c>
@@ -11549,8 +11933,12 @@
       <c r="AE98" s="3"/>
       <c r="AF98" s="3"/>
       <c r="AG98" s="3"/>
-      <c r="AH98" s="3"/>
-      <c r="AI98" s="3"/>
+      <c r="AH98" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI98" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ98" s="3">
         <v>100097</v>
       </c>
@@ -11628,8 +12016,12 @@
       <c r="AE99" s="3"/>
       <c r="AF99" s="3"/>
       <c r="AG99" s="3"/>
-      <c r="AH99" s="3"/>
-      <c r="AI99" s="3"/>
+      <c r="AH99" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI99" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ99" s="3">
         <v>100098</v>
       </c>
@@ -11717,8 +12109,12 @@
       <c r="AG100" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH100" s="3"/>
-      <c r="AI100" s="3"/>
+      <c r="AH100" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI100" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ100" s="3">
         <v>100099</v>
       </c>
@@ -11808,8 +12204,12 @@
       <c r="AG101" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH101" s="3"/>
-      <c r="AI101" s="3"/>
+      <c r="AH101" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI101" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ101" s="3">
         <v>100100</v>
       </c>
@@ -11885,8 +12285,12 @@
       <c r="AE102" s="3"/>
       <c r="AF102" s="3"/>
       <c r="AG102" s="3"/>
-      <c r="AH102" s="3"/>
-      <c r="AI102" s="3"/>
+      <c r="AH102" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI102" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ102" s="3">
         <v>100101</v>
       </c>
@@ -11974,8 +12378,12 @@
       <c r="AG103" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="AH103" s="3"/>
-      <c r="AI103" s="3"/>
+      <c r="AH103" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI103" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ103" s="3">
         <v>100102</v>
       </c>
@@ -12053,8 +12461,12 @@
       <c r="AG104" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH104" s="3"/>
-      <c r="AI104" s="3"/>
+      <c r="AH104" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI104" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ104" s="3">
         <v>100103</v>
       </c>
@@ -12130,8 +12542,12 @@
       <c r="AG105" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH105" s="3"/>
-      <c r="AI105" s="3"/>
+      <c r="AH105" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI105" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ105" s="3">
         <v>100104</v>
       </c>
@@ -12189,8 +12605,12 @@
       <c r="AG106" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH106" s="3"/>
-      <c r="AI106" s="3"/>
+      <c r="AH106" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI106" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ106" s="3">
         <v>100105</v>
       </c>
@@ -12266,8 +12686,12 @@
       <c r="AE107" s="3"/>
       <c r="AF107" s="3"/>
       <c r="AG107" s="3"/>
-      <c r="AH107" s="3"/>
-      <c r="AI107" s="3"/>
+      <c r="AH107" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI107" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ107" s="3">
         <v>100106</v>
       </c>
@@ -12359,8 +12783,12 @@
       <c r="AG108" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH108" s="3"/>
-      <c r="AI108" s="3"/>
+      <c r="AH108" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI108" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ108" s="3">
         <v>100107</v>
       </c>
@@ -12440,8 +12868,12 @@
       <c r="AG109" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH109" s="3"/>
-      <c r="AI109" s="3"/>
+      <c r="AH109" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI109" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ109" s="3">
         <v>100108</v>
       </c>
@@ -12517,8 +12949,12 @@
       <c r="AE110" s="3"/>
       <c r="AF110" s="3"/>
       <c r="AG110" s="3"/>
-      <c r="AH110" s="3"/>
-      <c r="AI110" s="3"/>
+      <c r="AH110" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI110" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ110" s="3">
         <v>100109</v>
       </c>
@@ -12598,8 +13034,12 @@
       <c r="AG111" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AH111" s="3"/>
-      <c r="AI111" s="3"/>
+      <c r="AH111" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI111" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ111" s="3">
         <v>100110</v>
       </c>
@@ -12687,8 +13127,12 @@
         <v>120</v>
       </c>
       <c r="AG112" s="3"/>
-      <c r="AH112" s="3"/>
-      <c r="AI112" s="3"/>
+      <c r="AH112" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI112" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ112" s="3">
         <v>100111</v>
       </c>
@@ -12768,8 +13212,12 @@
       <c r="AG113" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="AH113" s="3"/>
-      <c r="AI113" s="3"/>
+      <c r="AH113" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI113" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ113" s="3">
         <v>100112</v>
       </c>
@@ -12839,8 +13287,12 @@
       <c r="AG114" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="AH114" s="3"/>
-      <c r="AI114" s="3"/>
+      <c r="AH114" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI114" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ114" s="3">
         <v>100113</v>
       </c>
@@ -12934,8 +13386,12 @@
         <v>67</v>
       </c>
       <c r="AG115" s="3"/>
-      <c r="AH115" s="3"/>
-      <c r="AI115" s="3"/>
+      <c r="AH115" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI115" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ115" s="3">
         <v>100114</v>
       </c>
@@ -13023,8 +13479,12 @@
       <c r="AG116" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="AH116" s="3"/>
-      <c r="AI116" s="3"/>
+      <c r="AH116" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI116" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ116" s="3">
         <v>100115</v>
       </c>
@@ -13114,8 +13574,12 @@
       <c r="AG117" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH117" s="3"/>
-      <c r="AI117" s="3"/>
+      <c r="AH117" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI117" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ117" s="3">
         <v>100116</v>
       </c>
@@ -13197,8 +13661,12 @@
       <c r="AG118" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH118" s="3"/>
-      <c r="AI118" s="3"/>
+      <c r="AH118" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI118" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ118" s="3">
         <v>100117</v>
       </c>
@@ -13276,8 +13744,12 @@
       <c r="AG119" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AH119" s="3"/>
-      <c r="AI119" s="3"/>
+      <c r="AH119" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI119" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ119" s="3">
         <v>100118</v>
       </c>
@@ -13355,8 +13827,12 @@
         <v>64</v>
       </c>
       <c r="AG120" s="3"/>
-      <c r="AH120" s="3"/>
-      <c r="AI120" s="3"/>
+      <c r="AH120" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI120" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ120" s="3">
         <v>100119</v>
       </c>
@@ -13434,8 +13910,12 @@
       <c r="AE121" s="3"/>
       <c r="AF121" s="3"/>
       <c r="AG121" s="3"/>
-      <c r="AH121" s="3"/>
-      <c r="AI121" s="3"/>
+      <c r="AH121" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI121" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ121" s="3">
         <v>100120</v>
       </c>
@@ -13525,8 +14005,12 @@
       <c r="AG122" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH122" s="3"/>
-      <c r="AI122" s="3"/>
+      <c r="AH122" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI122" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ122" s="3">
         <v>100121</v>
       </c>
@@ -13604,8 +14088,12 @@
       <c r="AG123" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH123" s="3"/>
-      <c r="AI123" s="3"/>
+      <c r="AH123" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI123" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ123" s="3">
         <v>100122</v>
       </c>
@@ -13683,8 +14171,12 @@
         <v>90</v>
       </c>
       <c r="AG124" s="3"/>
-      <c r="AH124" s="3"/>
-      <c r="AI124" s="3"/>
+      <c r="AH124" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI124" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ124" s="3">
         <v>100123</v>
       </c>
@@ -13764,8 +14256,12 @@
       <c r="AG125" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH125" s="3"/>
-      <c r="AI125" s="3"/>
+      <c r="AH125" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI125" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ125" s="3">
         <v>100124</v>
       </c>
@@ -13845,8 +14341,12 @@
       <c r="AG126" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="AH126" s="3"/>
-      <c r="AI126" s="3"/>
+      <c r="AH126" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI126" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ126" s="3">
         <v>100125</v>
       </c>
@@ -13930,8 +14430,12 @@
       <c r="AG127" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="AH127" s="3"/>
-      <c r="AI127" s="3"/>
+      <c r="AH127" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI127" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ127" s="3">
         <v>100126</v>
       </c>
@@ -14009,8 +14513,12 @@
         <v>120</v>
       </c>
       <c r="AG128" s="3"/>
-      <c r="AH128" s="3"/>
-      <c r="AI128" s="3"/>
+      <c r="AH128" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI128" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ128" s="3">
         <v>100127</v>
       </c>
@@ -14088,8 +14596,12 @@
         <v>120</v>
       </c>
       <c r="AG129" s="3"/>
-      <c r="AH129" s="3"/>
-      <c r="AI129" s="3"/>
+      <c r="AH129" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI129" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ129" s="3">
         <v>100128</v>
       </c>
@@ -14175,8 +14687,12 @@
       </c>
       <c r="AF130" s="3"/>
       <c r="AG130" s="3"/>
-      <c r="AH130" s="3"/>
-      <c r="AI130" s="3"/>
+      <c r="AH130" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI130" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ130" s="3">
         <v>100129</v>
       </c>
@@ -14266,8 +14782,12 @@
       <c r="AG131" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH131" s="3"/>
-      <c r="AI131" s="3"/>
+      <c r="AH131" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI131" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ131" s="3">
         <v>100130</v>
       </c>
@@ -14347,8 +14867,12 @@
       <c r="AG132" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="AH132" s="3"/>
-      <c r="AI132" s="3"/>
+      <c r="AH132" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI132" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ132" s="3">
         <v>100131</v>
       </c>
@@ -14436,8 +14960,12 @@
       <c r="AG133" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH133" s="3"/>
-      <c r="AI133" s="3"/>
+      <c r="AH133" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI133" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ133" s="3">
         <v>100132</v>
       </c>
@@ -14513,8 +15041,12 @@
       <c r="AE134" s="3"/>
       <c r="AF134" s="3"/>
       <c r="AG134" s="3"/>
-      <c r="AH134" s="3"/>
-      <c r="AI134" s="3"/>
+      <c r="AH134" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI134" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ134" s="3">
         <v>100133</v>
       </c>
@@ -14594,8 +15126,12 @@
       <c r="AG135" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="AH135" s="3"/>
-      <c r="AI135" s="3"/>
+      <c r="AH135" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI135" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ135" s="3">
         <v>100134</v>
       </c>
@@ -14675,8 +15211,12 @@
       <c r="AE136" s="3"/>
       <c r="AF136" s="3"/>
       <c r="AG136" s="3"/>
-      <c r="AH136" s="3"/>
-      <c r="AI136" s="3"/>
+      <c r="AH136" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI136" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ136" s="3">
         <v>100135</v>
       </c>
@@ -14764,8 +15304,12 @@
       <c r="AG137" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH137" s="3"/>
-      <c r="AI137" s="3"/>
+      <c r="AH137" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI137" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ137" s="3">
         <v>100136</v>
       </c>
@@ -14845,8 +15389,12 @@
       <c r="AG138" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH138" s="3"/>
-      <c r="AI138" s="3"/>
+      <c r="AH138" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI138" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ138" s="3">
         <v>100137</v>
       </c>
@@ -14934,8 +15482,12 @@
       <c r="AG139" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH139" s="3"/>
-      <c r="AI139" s="3"/>
+      <c r="AH139" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI139" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ139" s="3">
         <v>100138</v>
       </c>
@@ -15015,8 +15567,12 @@
       <c r="AG140" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AH140" s="3"/>
-      <c r="AI140" s="3"/>
+      <c r="AH140" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI140" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ140" s="3">
         <v>100139</v>
       </c>
@@ -15090,8 +15646,12 @@
       </c>
       <c r="AF141" s="3"/>
       <c r="AG141" s="3"/>
-      <c r="AH141" s="3"/>
-      <c r="AI141" s="3"/>
+      <c r="AH141" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI141" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ141" s="3">
         <v>100140</v>
       </c>
@@ -15183,8 +15743,12 @@
       <c r="AG142" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH142" s="3"/>
-      <c r="AI142" s="3"/>
+      <c r="AH142" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI142" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ142" s="3">
         <v>100141</v>
       </c>
@@ -15254,8 +15818,12 @@
         <v>64</v>
       </c>
       <c r="AG143" s="3"/>
-      <c r="AH143" s="3"/>
-      <c r="AI143" s="3"/>
+      <c r="AH143" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI143" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ143" s="3">
         <v>100142</v>
       </c>
@@ -15345,8 +15913,12 @@
       <c r="AG144" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AH144" s="3"/>
-      <c r="AI144" s="3"/>
+      <c r="AH144" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI144" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ144" s="3">
         <v>100143</v>
       </c>
@@ -15438,8 +16010,12 @@
       <c r="AG145" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH145" s="3"/>
-      <c r="AI145" s="3"/>
+      <c r="AH145" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI145" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ145" s="3">
         <v>100144</v>
       </c>
@@ -15523,8 +16099,12 @@
       <c r="AG146" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="AH146" s="3"/>
-      <c r="AI146" s="3"/>
+      <c r="AH146" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI146" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ146" s="3">
         <v>100145</v>
       </c>
@@ -15596,8 +16176,12 @@
       <c r="AG147" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="AH147" s="3"/>
-      <c r="AI147" s="3"/>
+      <c r="AH147" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI147" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ147" s="3">
         <v>100146</v>
       </c>
@@ -15677,8 +16261,12 @@
       <c r="AG148" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH148" s="3"/>
-      <c r="AI148" s="3"/>
+      <c r="AH148" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI148" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ148" s="3">
         <v>100147</v>
       </c>
@@ -15760,8 +16348,12 @@
       <c r="AG149" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH149" s="3"/>
-      <c r="AI149" s="3"/>
+      <c r="AH149" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI149" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ149" s="3">
         <v>100148</v>
       </c>
@@ -15831,8 +16423,12 @@
       <c r="AG150" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH150" s="3"/>
-      <c r="AI150" s="3"/>
+      <c r="AH150" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI150" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ150" s="3">
         <v>100149</v>
       </c>
@@ -15898,8 +16494,12 @@
         <v>339</v>
       </c>
       <c r="AG151" s="3"/>
-      <c r="AH151" s="3"/>
-      <c r="AI151" s="3"/>
+      <c r="AH151" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI151" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ151" s="3">
         <v>100150</v>
       </c>
@@ -15995,8 +16595,12 @@
       <c r="AG152" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="AH152" s="3"/>
-      <c r="AI152" s="3"/>
+      <c r="AH152" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI152" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ152" s="3">
         <v>100151</v>
       </c>
@@ -16064,8 +16668,12 @@
       <c r="AG153" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="AH153" s="3"/>
-      <c r="AI153" s="3"/>
+      <c r="AH153" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI153" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ153" s="3">
         <v>100152</v>
       </c>
@@ -16129,8 +16737,12 @@
         <v>67</v>
       </c>
       <c r="AG154" s="3"/>
-      <c r="AH154" s="3"/>
-      <c r="AI154" s="3"/>
+      <c r="AH154" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI154" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ154" s="3">
         <v>100153</v>
       </c>
@@ -16226,8 +16838,12 @@
       <c r="AG155" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH155" s="3"/>
-      <c r="AI155" s="3"/>
+      <c r="AH155" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI155" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ155" s="3">
         <v>100154</v>
       </c>
@@ -16315,8 +16931,12 @@
       <c r="AG156" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="AH156" s="3"/>
-      <c r="AI156" s="3"/>
+      <c r="AH156" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI156" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ156" s="3">
         <v>100155</v>
       </c>
@@ -16408,8 +17028,12 @@
       <c r="AG157" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="AH157" s="3"/>
-      <c r="AI157" s="3"/>
+      <c r="AH157" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI157" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ157" s="3">
         <v>100156</v>
       </c>
@@ -16485,8 +17109,12 @@
       <c r="AE158" s="3"/>
       <c r="AF158" s="3"/>
       <c r="AG158" s="3"/>
-      <c r="AH158" s="3"/>
-      <c r="AI158" s="3"/>
+      <c r="AH158" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI158" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ158" s="3">
         <v>100157</v>
       </c>
@@ -16580,8 +17208,12 @@
       <c r="AG159" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH159" s="3"/>
-      <c r="AI159" s="3"/>
+      <c r="AH159" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI159" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ159" s="3">
         <v>100158</v>
       </c>
@@ -16657,8 +17289,12 @@
       <c r="AG160" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="AH160" s="3"/>
-      <c r="AI160" s="3"/>
+      <c r="AH160" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI160" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ160" s="3">
         <v>100159</v>
       </c>
@@ -16750,8 +17386,12 @@
       <c r="AG161" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH161" s="3"/>
-      <c r="AI161" s="3"/>
+      <c r="AH161" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI161" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ161" s="3">
         <v>100160</v>
       </c>
@@ -16835,8 +17475,12 @@
       </c>
       <c r="AF162" s="3"/>
       <c r="AG162" s="3"/>
-      <c r="AH162" s="3"/>
-      <c r="AI162" s="3"/>
+      <c r="AH162" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI162" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ162" s="3">
         <v>100161</v>
       </c>
@@ -16928,8 +17572,12 @@
       <c r="AG163" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH163" s="3"/>
-      <c r="AI163" s="3"/>
+      <c r="AH163" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI163" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ163" s="3">
         <v>100162</v>
       </c>
@@ -17021,8 +17669,12 @@
       <c r="AG164" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH164" s="3"/>
-      <c r="AI164" s="3"/>
+      <c r="AH164" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI164" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ164" s="3">
         <v>100163</v>
       </c>
@@ -17102,8 +17754,12 @@
       <c r="AG165" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH165" s="3"/>
-      <c r="AI165" s="3"/>
+      <c r="AH165" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI165" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ165" s="3">
         <v>100164</v>
       </c>
@@ -17185,8 +17841,12 @@
       <c r="AG166" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="AH166" s="3"/>
-      <c r="AI166" s="3"/>
+      <c r="AH166" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI166" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ166" s="3">
         <v>100165</v>
       </c>
@@ -17262,8 +17922,12 @@
       <c r="AE167" s="3"/>
       <c r="AF167" s="3"/>
       <c r="AG167" s="3"/>
-      <c r="AH167" s="3"/>
-      <c r="AI167" s="3"/>
+      <c r="AH167" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI167" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ167" s="3">
         <v>100166</v>
       </c>
@@ -17339,8 +18003,12 @@
       <c r="AE168" s="3"/>
       <c r="AF168" s="3"/>
       <c r="AG168" s="3"/>
-      <c r="AH168" s="3"/>
-      <c r="AI168" s="3"/>
+      <c r="AH168" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI168" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ168" s="3">
         <v>100167</v>
       </c>
@@ -17428,8 +18096,12 @@
       <c r="AG169" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="AH169" s="3"/>
-      <c r="AI169" s="3"/>
+      <c r="AH169" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI169" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ169" s="3">
         <v>100168</v>
       </c>
@@ -17511,8 +18183,12 @@
       <c r="AG170" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH170" s="3"/>
-      <c r="AI170" s="3"/>
+      <c r="AH170" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI170" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ170" s="3">
         <v>100169</v>
       </c>
@@ -17594,8 +18270,12 @@
       <c r="AG171" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH171" s="3"/>
-      <c r="AI171" s="3"/>
+      <c r="AH171" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI171" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ171" s="3">
         <v>100170</v>
       </c>
@@ -17665,8 +18345,12 @@
       <c r="AG172" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="AH172" s="3"/>
-      <c r="AI172" s="3"/>
+      <c r="AH172" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI172" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ172" s="3">
         <v>100171</v>
       </c>
@@ -17748,8 +18432,12 @@
       <c r="AG173" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH173" s="3"/>
-      <c r="AI173" s="3"/>
+      <c r="AH173" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI173" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ173" s="3">
         <v>100172</v>
       </c>
@@ -17837,8 +18525,12 @@
       <c r="AG174" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH174" s="3"/>
-      <c r="AI174" s="3"/>
+      <c r="AH174" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI174" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ174" s="3">
         <v>100173</v>
       </c>
@@ -17930,8 +18622,12 @@
       <c r="AG175" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH175" s="3"/>
-      <c r="AI175" s="3"/>
+      <c r="AH175" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI175" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ175" s="3">
         <v>100174</v>
       </c>
@@ -18009,8 +18705,12 @@
         <v>120</v>
       </c>
       <c r="AG176" s="3"/>
-      <c r="AH176" s="3"/>
-      <c r="AI176" s="3"/>
+      <c r="AH176" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI176" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ176" s="3">
         <v>100175</v>
       </c>
@@ -18086,8 +18786,12 @@
       <c r="AG177" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="AH177" s="3"/>
-      <c r="AI177" s="3"/>
+      <c r="AH177" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI177" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ177" s="3">
         <v>100176</v>
       </c>
@@ -18159,8 +18863,12 @@
       <c r="AG178" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="AH178" s="3"/>
-      <c r="AI178" s="3"/>
+      <c r="AH178" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI178" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ178" s="3">
         <v>100177</v>
       </c>
@@ -18250,8 +18958,12 @@
       <c r="AG179" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH179" s="3"/>
-      <c r="AI179" s="3"/>
+      <c r="AH179" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI179" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ179" s="3">
         <v>100178</v>
       </c>
@@ -18327,8 +19039,12 @@
       <c r="AE180" s="3"/>
       <c r="AF180" s="3"/>
       <c r="AG180" s="3"/>
-      <c r="AH180" s="3"/>
-      <c r="AI180" s="3"/>
+      <c r="AH180" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI180" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ180" s="3">
         <v>100179</v>
       </c>
@@ -18422,8 +19138,12 @@
       <c r="AG181" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH181" s="3"/>
-      <c r="AI181" s="3"/>
+      <c r="AH181" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI181" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ181" s="3">
         <v>100180</v>
       </c>
@@ -18515,8 +19235,12 @@
       <c r="AG182" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH182" s="3"/>
-      <c r="AI182" s="3"/>
+      <c r="AH182" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI182" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ182" s="3">
         <v>100181</v>
       </c>
@@ -18609,7 +19333,9 @@
         <v>49</v>
       </c>
       <c r="AH183" s="3"/>
-      <c r="AI183" s="3"/>
+      <c r="AI183" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ183" s="3">
         <v>100182</v>
       </c>
@@ -18634,8 +19360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F0A42D-5D3A-4094-B0B2-F7408DD7A1F0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.8" x14ac:dyDescent="0.3"/>

</xml_diff>